<commit_message>
chapter potencjalne problemy modified
</commit_message>
<xml_diff>
--- a/meas/Measurements_v3.xlsx
+++ b/meas/Measurements_v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\RF_VLF_SAQ_Reception\meas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E5D2A60-89BC-4D93-BFEB-8B73992C1F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A8791D4-1353-4F96-B847-9690F79C7768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{CB450F67-C83A-4305-ACBC-60FD295E7ED8}"/>
+    <workbookView xWindow="7905" yWindow="4995" windowWidth="20895" windowHeight="10470" activeTab="1" xr2:uid="{CB450F67-C83A-4305-ACBC-60FD295E7ED8}"/>
   </bookViews>
   <sheets>
     <sheet name="Resonance_frequency" sheetId="1" r:id="rId1"/>
@@ -228,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -246,20 +246,18 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -646,6 +644,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-3D00-4A33-B4FF-D1DDA116212F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:xVal>
             <c:numRef>
@@ -728,6 +731,9 @@
               <c:delete val="1"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-3D00-4A33-B4FF-D1DDA116212F}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -855,6 +861,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-3D00-4A33-B4FF-D1DDA116212F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:dLbl>
@@ -873,6 +884,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-3D00-4A33-B4FF-D1DDA116212F}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -880,6 +894,9 @@
               <c:delete val="1"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-3D00-4A33-B4FF-D1DDA116212F}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -1017,6 +1034,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-3D00-4A33-B4FF-D1DDA116212F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:dLbl>
@@ -1035,6 +1057,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-3D00-4A33-B4FF-D1DDA116212F}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1042,6 +1067,9 @@
               <c:delete val="1"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-3D00-4A33-B4FF-D1DDA116212F}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -2109,7 +2137,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="pl-PL" sz="1100" baseline="0"/>
-            <a:t> - 17.26kHz = 210kHz </a:t>
+            <a:t> - 17.26kHz = 210Hz </a:t>
           </a:r>
           <a:endParaRPr lang="pl-PL" sz="1100"/>
         </a:p>
@@ -2539,13 +2567,13 @@
   <dimension ref="B2:Y46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="O3" workbookViewId="0">
-      <selection activeCell="AM1" sqref="AM1"/>
+      <selection activeCell="V12" sqref="V12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="10.85546875" customWidth="1"/>
-    <col min="18" max="18" width="9.140625" style="15"/>
+    <col min="18" max="18" width="9.140625" style="12"/>
     <col min="19" max="19" width="10.85546875" customWidth="1"/>
     <col min="20" max="20" width="23" customWidth="1"/>
     <col min="21" max="21" width="13.28515625" customWidth="1"/>
@@ -2582,7 +2610,7 @@
       <c r="B8" t="s">
         <v>5</v>
       </c>
-      <c r="R8" s="15" t="s">
+      <c r="R8" s="12" t="s">
         <v>12</v>
       </c>
       <c r="S8" t="s">
@@ -2600,14 +2628,14 @@
       </c>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="R9" s="15">
+      <c r="R9" s="12">
         <v>5</v>
       </c>
       <c r="S9" s="2">
         <v>-101.2</v>
       </c>
-      <c r="T9" s="13">
-        <f>S9-$S$28</f>
+      <c r="T9" s="2">
+        <f t="shared" ref="T9:T41" si="0">S9-$S$28</f>
         <v>-68.5</v>
       </c>
       <c r="U9" s="2"/>
@@ -2620,14 +2648,14 @@
       </c>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="R10" s="15">
+      <c r="R10" s="12">
         <v>6</v>
       </c>
       <c r="S10" s="2">
         <v>-95</v>
       </c>
-      <c r="T10" s="13">
-        <f>S10-$S$28</f>
+      <c r="T10" s="2">
+        <f t="shared" si="0"/>
         <v>-62.3</v>
       </c>
       <c r="U10" s="2"/>
@@ -2636,27 +2664,27 @@
       <c r="B11" t="s">
         <v>13</v>
       </c>
-      <c r="R11" s="15">
+      <c r="R11" s="12">
         <v>7</v>
       </c>
       <c r="S11" s="2">
         <v>-90</v>
       </c>
-      <c r="T11" s="13">
-        <f>S11-$S$28</f>
+      <c r="T11" s="2">
+        <f t="shared" si="0"/>
         <v>-57.3</v>
       </c>
       <c r="U11" s="2"/>
     </row>
     <row r="12" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="R12" s="15">
+      <c r="R12" s="12">
         <v>8</v>
       </c>
       <c r="S12" s="2">
         <v>-85.9</v>
       </c>
-      <c r="T12" s="13">
-        <f>S12-$S$28</f>
+      <c r="T12" s="2">
+        <f t="shared" si="0"/>
         <v>-53.2</v>
       </c>
       <c r="U12" s="2"/>
@@ -2667,125 +2695,125 @@
       <c r="B13" t="s">
         <v>7</v>
       </c>
-      <c r="R13" s="16">
+      <c r="R13" s="12">
         <v>9</v>
       </c>
-      <c r="S13" s="13">
+      <c r="S13" s="2">
         <v>-82.1</v>
       </c>
-      <c r="T13" s="13">
-        <f>S13-$S$28</f>
+      <c r="T13" s="2">
+        <f t="shared" si="0"/>
         <v>-49.399999999999991</v>
       </c>
-      <c r="U13" s="13"/>
+      <c r="U13" s="2"/>
       <c r="W13" s="2"/>
       <c r="X13" s="2"/>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="R14" s="16">
+      <c r="R14" s="12">
         <v>10</v>
       </c>
-      <c r="S14" s="13">
+      <c r="S14" s="2">
         <v>-78.8</v>
       </c>
-      <c r="T14" s="13">
-        <f>S14-$S$28</f>
+      <c r="T14" s="2">
+        <f t="shared" si="0"/>
         <v>-46.099999999999994</v>
       </c>
-      <c r="U14" s="13"/>
+      <c r="U14" s="2"/>
     </row>
     <row r="15" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>28</v>
       </c>
-      <c r="R15" s="16">
+      <c r="R15" s="12">
         <v>11</v>
       </c>
-      <c r="S15" s="13">
+      <c r="S15" s="2">
         <v>-75.7</v>
       </c>
-      <c r="T15" s="13">
-        <f>S15-$S$28</f>
+      <c r="T15" s="2">
+        <f t="shared" si="0"/>
         <v>-43</v>
       </c>
-      <c r="U15" s="13"/>
+      <c r="U15" s="2"/>
     </row>
     <row r="16" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>30</v>
       </c>
-      <c r="R16" s="16">
+      <c r="R16" s="12">
         <v>12</v>
       </c>
-      <c r="S16" s="13">
+      <c r="S16" s="2">
         <v>-72.7</v>
       </c>
-      <c r="T16" s="13">
-        <f>S16-$S$28</f>
+      <c r="T16" s="2">
+        <f t="shared" si="0"/>
         <v>-40</v>
       </c>
-      <c r="U16" s="13"/>
+      <c r="U16" s="2"/>
     </row>
     <row r="17" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>31</v>
       </c>
-      <c r="R17" s="16">
+      <c r="R17" s="12">
         <v>13</v>
       </c>
-      <c r="S17" s="13">
+      <c r="S17" s="2">
         <v>-69.5</v>
       </c>
-      <c r="T17" s="13">
-        <f>S17-$S$28</f>
+      <c r="T17" s="2">
+        <f t="shared" si="0"/>
         <v>-36.799999999999997</v>
       </c>
-      <c r="U17" s="13"/>
+      <c r="U17" s="2"/>
     </row>
     <row r="18" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="R18" s="16">
+      <c r="R18" s="12">
         <v>14</v>
       </c>
-      <c r="S18" s="13">
+      <c r="S18" s="2">
         <v>-66.2</v>
       </c>
-      <c r="T18" s="13">
-        <f>S18-$S$28</f>
+      <c r="T18" s="2">
+        <f t="shared" si="0"/>
         <v>-33.5</v>
       </c>
-      <c r="U18" s="13"/>
+      <c r="U18" s="2"/>
     </row>
     <row r="19" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>29</v>
       </c>
-      <c r="R19" s="16">
+      <c r="R19" s="12">
         <v>15</v>
       </c>
-      <c r="S19" s="13">
+      <c r="S19" s="2">
         <v>-62.1</v>
       </c>
-      <c r="T19" s="13">
-        <f>S19-$S$28</f>
+      <c r="T19" s="2">
+        <f t="shared" si="0"/>
         <v>-29.4</v>
       </c>
-      <c r="U19" s="13"/>
+      <c r="U19" s="2"/>
     </row>
     <row r="20" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="R20" s="16">
+      <c r="R20" s="12">
         <v>16</v>
       </c>
-      <c r="S20" s="13">
+      <c r="S20" s="2">
         <v>-56.5</v>
       </c>
-      <c r="T20" s="13">
-        <f>S20-$S$28</f>
+      <c r="T20" s="2">
+        <f t="shared" si="0"/>
         <v>-23.799999999999997</v>
       </c>
-      <c r="U20" s="13"/>
+      <c r="U20" s="2"/>
       <c r="W20" t="s">
         <v>2</v>
       </c>
@@ -2794,17 +2822,17 @@
       <c r="B21" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="R21" s="16">
+      <c r="R21" s="12">
         <v>16.8</v>
       </c>
-      <c r="S21" s="13">
+      <c r="S21" s="2">
         <v>-48.4</v>
       </c>
-      <c r="T21" s="13">
-        <f>S21-$S$28</f>
+      <c r="T21" s="2">
+        <f t="shared" si="0"/>
         <v>-15.699999999999996</v>
       </c>
-      <c r="U21" s="13"/>
+      <c r="U21" s="2"/>
       <c r="W21" s="2">
         <v>17.399999999999999</v>
       </c>
@@ -2816,17 +2844,17 @@
       <c r="B22" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="R22" s="16">
+      <c r="R22" s="12">
         <v>16.899999999999999</v>
       </c>
-      <c r="S22" s="13">
+      <c r="S22" s="2">
         <v>-46.5</v>
       </c>
-      <c r="T22" s="13">
-        <f>S22-$S$28</f>
+      <c r="T22" s="2">
+        <f t="shared" si="0"/>
         <v>-13.799999999999997</v>
       </c>
-      <c r="U22" s="13"/>
+      <c r="U22" s="2"/>
       <c r="W22" s="2">
         <v>17.399999999999999</v>
       </c>
@@ -2835,49 +2863,49 @@
       </c>
     </row>
     <row r="23" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="R23" s="16">
+      <c r="R23" s="12">
         <v>17</v>
       </c>
-      <c r="S23" s="13">
+      <c r="S23" s="2">
         <v>-44.6</v>
       </c>
-      <c r="T23" s="13">
-        <f>S23-$S$28</f>
+      <c r="T23" s="2">
+        <f t="shared" si="0"/>
         <v>-11.899999999999999</v>
       </c>
-      <c r="U23" s="13"/>
+      <c r="U23" s="2"/>
     </row>
     <row r="24" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="R24" s="16">
+      <c r="R24" s="12">
         <v>17.100000000000001</v>
       </c>
-      <c r="S24" s="13">
+      <c r="S24" s="2">
         <v>-42</v>
       </c>
-      <c r="T24" s="13">
-        <f>S24-$S$28</f>
+      <c r="T24" s="2">
+        <f t="shared" si="0"/>
         <v>-9.2999999999999972</v>
       </c>
-      <c r="U24" s="13"/>
+      <c r="U24" s="2"/>
       <c r="W24" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="25" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="R25" s="16">
+      <c r="R25" s="12">
         <v>17.2</v>
       </c>
-      <c r="S25" s="13">
+      <c r="S25" s="2">
         <v>-38.5</v>
       </c>
-      <c r="T25" s="13">
-        <f>S25-$S$28</f>
+      <c r="T25" s="2">
+        <f t="shared" si="0"/>
         <v>-5.7999999999999972</v>
       </c>
-      <c r="U25" s="13"/>
+      <c r="U25" s="2"/>
       <c r="W25" s="2">
         <v>17.260999999999999</v>
       </c>
@@ -2889,18 +2917,18 @@
       <c r="B26" t="s">
         <v>10</v>
       </c>
-      <c r="R26" s="18">
+      <c r="R26" s="14">
         <v>17.260999999999999</v>
       </c>
-      <c r="S26" s="19">
+      <c r="S26" s="15">
         <f>S28-3</f>
         <v>-35.700000000000003</v>
       </c>
-      <c r="T26" s="19">
-        <f>S26-$S$28</f>
+      <c r="T26" s="15">
+        <f t="shared" si="0"/>
         <v>-3</v>
       </c>
-      <c r="U26" s="20">
+      <c r="U26" s="18">
         <f>R29-R26</f>
         <v>0.20599999999999952</v>
       </c>
@@ -2912,50 +2940,50 @@
       </c>
     </row>
     <row r="27" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="R27" s="16">
+      <c r="R27" s="12">
         <v>17.3</v>
       </c>
-      <c r="S27" s="13">
+      <c r="S27" s="2">
         <v>-34</v>
       </c>
-      <c r="T27" s="13">
-        <f>S27-$S$28</f>
+      <c r="T27" s="2">
+        <f t="shared" si="0"/>
         <v>-1.2999999999999972</v>
       </c>
-      <c r="U27" s="20"/>
+      <c r="U27" s="18"/>
     </row>
     <row r="28" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>14</v>
       </c>
-      <c r="R28" s="17">
+      <c r="R28" s="13">
         <v>17.399999999999999</v>
       </c>
-      <c r="S28" s="14">
+      <c r="S28" s="11">
         <v>-32.700000000000003</v>
       </c>
-      <c r="T28" s="14">
-        <f>S28-$S$28</f>
+      <c r="T28" s="11">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U28" s="20"/>
+      <c r="U28" s="18"/>
       <c r="W28" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="29" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="R29" s="18">
+      <c r="R29" s="14">
         <v>17.466999999999999</v>
       </c>
-      <c r="S29" s="19">
+      <c r="S29" s="15">
         <f>S28-3</f>
         <v>-35.700000000000003</v>
       </c>
-      <c r="T29" s="19">
-        <f>S29-$S$28</f>
+      <c r="T29" s="15">
+        <f t="shared" si="0"/>
         <v>-3</v>
       </c>
-      <c r="U29" s="20"/>
+      <c r="U29" s="18"/>
       <c r="W29" s="2">
         <v>17.466999999999999</v>
       </c>
@@ -2967,17 +2995,17 @@
       <c r="B30" t="s">
         <v>15</v>
       </c>
-      <c r="R30" s="16">
+      <c r="R30" s="12">
         <v>17.5</v>
       </c>
-      <c r="S30" s="13">
+      <c r="S30" s="2">
         <v>-37</v>
       </c>
-      <c r="T30" s="13">
-        <f>S30-$S$28</f>
+      <c r="T30" s="2">
+        <f t="shared" si="0"/>
         <v>-4.2999999999999972</v>
       </c>
-      <c r="U30" s="13"/>
+      <c r="U30" s="2"/>
       <c r="W30" s="2">
         <v>17.466999999999999</v>
       </c>
@@ -2986,17 +3014,17 @@
       </c>
     </row>
     <row r="31" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="R31" s="16">
+      <c r="R31" s="12">
         <v>18</v>
       </c>
-      <c r="S31" s="13">
+      <c r="S31" s="2">
         <v>-48.5</v>
       </c>
-      <c r="T31" s="13">
-        <f>S31-$S$28</f>
+      <c r="T31" s="2">
+        <f t="shared" si="0"/>
         <v>-15.799999999999997</v>
       </c>
-      <c r="U31" s="13"/>
+      <c r="U31" s="2"/>
       <c r="W31" s="2"/>
       <c r="X31" s="2"/>
     </row>
@@ -3004,146 +3032,146 @@
       <c r="B32" t="s">
         <v>36</v>
       </c>
-      <c r="R32" s="16">
+      <c r="R32" s="12">
         <v>19</v>
       </c>
-      <c r="S32" s="13">
+      <c r="S32" s="2">
         <v>-56.4</v>
       </c>
-      <c r="T32" s="13">
-        <f>S32-$S$28</f>
+      <c r="T32" s="2">
+        <f t="shared" si="0"/>
         <v>-23.699999999999996</v>
       </c>
-      <c r="U32" s="13"/>
+      <c r="U32" s="2"/>
     </row>
     <row r="33" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="R33" s="16">
+      <c r="R33" s="12">
         <v>20</v>
       </c>
-      <c r="S33" s="13">
+      <c r="S33" s="2">
         <v>-59.9</v>
       </c>
-      <c r="T33" s="13">
-        <f>S33-$S$28</f>
+      <c r="T33" s="2">
+        <f t="shared" si="0"/>
         <v>-27.199999999999996</v>
       </c>
-      <c r="U33" s="13"/>
-      <c r="V33" s="15"/>
+      <c r="U33" s="2"/>
+      <c r="V33" s="12"/>
     </row>
     <row r="34" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>11</v>
       </c>
-      <c r="R34" s="16">
+      <c r="R34" s="12">
         <v>21</v>
       </c>
-      <c r="S34" s="13">
+      <c r="S34" s="2">
         <v>-62.3</v>
       </c>
-      <c r="T34" s="13">
-        <f>S34-$S$28</f>
+      <c r="T34" s="2">
+        <f t="shared" si="0"/>
         <v>-29.599999999999994</v>
       </c>
-      <c r="U34" s="13"/>
+      <c r="U34" s="2"/>
     </row>
     <row r="35" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="R35" s="16">
+      <c r="R35" s="12">
         <v>22</v>
       </c>
-      <c r="S35" s="13">
+      <c r="S35" s="2">
         <v>-64.099999999999994</v>
       </c>
-      <c r="T35" s="13">
-        <f>S35-$S$28</f>
+      <c r="T35" s="2">
+        <f t="shared" si="0"/>
         <v>-31.399999999999991</v>
       </c>
-      <c r="U35" s="13"/>
+      <c r="U35" s="2"/>
     </row>
     <row r="36" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>34</v>
       </c>
-      <c r="R36" s="16">
+      <c r="R36" s="12">
         <v>23</v>
       </c>
-      <c r="S36" s="13">
+      <c r="S36" s="2">
         <v>-65.5</v>
       </c>
-      <c r="T36" s="13">
-        <f>S36-$S$28</f>
+      <c r="T36" s="2">
+        <f t="shared" si="0"/>
         <v>-32.799999999999997</v>
       </c>
-      <c r="U36" s="13"/>
-      <c r="X36" s="11"/>
-      <c r="Y36" s="12"/>
+      <c r="U36" s="2"/>
+      <c r="X36" s="16"/>
+      <c r="Y36" s="17"/>
     </row>
     <row r="37" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>35</v>
       </c>
-      <c r="R37" s="15">
+      <c r="R37" s="12">
         <v>24</v>
       </c>
       <c r="S37" s="2">
         <v>-66.599999999999994</v>
       </c>
-      <c r="T37" s="13">
-        <f>S37-$S$28</f>
+      <c r="T37" s="2">
+        <f t="shared" si="0"/>
         <v>-33.899999999999991</v>
       </c>
-      <c r="U37" s="13"/>
+      <c r="U37" s="2"/>
       <c r="X37" s="3"/>
       <c r="Y37" s="3"/>
     </row>
     <row r="38" spans="2:25" x14ac:dyDescent="0.25">
       <c r="F38" s="2"/>
-      <c r="R38" s="15">
+      <c r="R38" s="12">
         <v>25</v>
       </c>
       <c r="S38" s="2">
         <v>-67.7</v>
       </c>
-      <c r="T38" s="13">
-        <f>S38-$S$28</f>
+      <c r="T38" s="2">
+        <f t="shared" si="0"/>
         <v>-35</v>
       </c>
-      <c r="U38" s="13"/>
+      <c r="U38" s="2"/>
     </row>
     <row r="39" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="R39" s="15">
+      <c r="R39" s="12">
         <v>26</v>
       </c>
       <c r="S39" s="2">
         <v>-68.5</v>
       </c>
-      <c r="T39" s="13">
-        <f>S39-$S$28</f>
+      <c r="T39" s="2">
+        <f t="shared" si="0"/>
         <v>-35.799999999999997</v>
       </c>
       <c r="U39" s="2"/>
     </row>
     <row r="40" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="R40" s="15">
+      <c r="R40" s="12">
         <v>27</v>
       </c>
       <c r="S40" s="2">
         <v>-69.5</v>
       </c>
-      <c r="T40" s="13">
-        <f>S40-$S$28</f>
+      <c r="T40" s="2">
+        <f t="shared" si="0"/>
         <v>-36.799999999999997</v>
       </c>
       <c r="U40" s="2"/>
     </row>
     <row r="41" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="R41" s="15">
+      <c r="R41" s="12">
         <v>28</v>
       </c>
       <c r="S41" s="2">
         <v>-70</v>
       </c>
-      <c r="T41" s="13">
-        <f>S41-$S$28</f>
+      <c r="T41" s="2">
+        <f t="shared" si="0"/>
         <v>-37.299999999999997</v>
       </c>
       <c r="U41" s="2"/>

</xml_diff>